<commit_message>
Fixed uploading xml bug, added latest menu items
</commit_message>
<xml_diff>
--- a/website/docs/menu.xlsx
+++ b/website/docs/menu.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
   <si>
     <t>Maandag</t>
   </si>
@@ -50,34 +50,15 @@
     <t>Combi deal</t>
   </si>
   <si>
-    <t>Ambachtelijke soep
-Dag special</t>
-  </si>
-  <si>
     <t>Wok to go</t>
   </si>
   <si>
-    <t>€ 3,25
-€ 1,65</t>
-  </si>
-  <si>
-    <t>€ 2,50
-€ 1,29</t>
-  </si>
-  <si>
-    <t>€ 1,99
-€ 2,39</t>
-  </si>
-  <si>
     <t>3.75</t>
   </si>
   <si>
     <t>soep van de dag</t>
   </si>
   <si>
-    <t>€ 1.49</t>
-  </si>
-  <si>
     <t>Portie patat</t>
   </si>
   <si>
@@ -228,112 +209,106 @@
     <t>kippen soep met stokbrood en kruiden boter.</t>
   </si>
   <si>
-    <t>€ 3.49
-€ 1,79</t>
-  </si>
-  <si>
-    <t>home made gehaktbal</t>
-  </si>
-  <si>
-    <t>vismarkt</t>
-  </si>
-  <si>
-    <t>groente bouillon</t>
-  </si>
-  <si>
-    <t>bospaddestoelen bouillon</t>
-  </si>
-  <si>
-    <t>week 12 van 16 maart t/m 20 maart 2015.</t>
-  </si>
-  <si>
-    <t>broodje room pate met cranberry compote</t>
-  </si>
-  <si>
-    <t>broodje rosbief met pesto &amp; pijnboom pitjes</t>
-  </si>
-  <si>
-    <t>broodje italiaanse rauwe ham met ei en verse tuinkruiden</t>
-  </si>
-  <si>
-    <t>wrap met roomkas rucola en gerookte zalm</t>
-  </si>
-  <si>
-    <t>broodje runder ossenworst</t>
-  </si>
-  <si>
-    <t>broodje sambal kaas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> broodje oude leidse</t>
-  </si>
-  <si>
-    <t>broodje emmentaler</t>
-  </si>
-  <si>
-    <t>broodje roquefort met appelstroop</t>
-  </si>
-  <si>
-    <t>geitenkaas tomaat</t>
-  </si>
-  <si>
-    <t>wijn cervelaat met kaas tomaat en komkommer</t>
-  </si>
-  <si>
-    <t>choriso kaas</t>
-  </si>
-  <si>
-    <t>roombrie</t>
-  </si>
-  <si>
-    <t>turkse pizza met ijsberg sla en knoflooksaus</t>
-  </si>
-  <si>
-    <t>omelet van de plaat</t>
-  </si>
-  <si>
-    <t>lasagne bolognaise</t>
-  </si>
-  <si>
-    <t>gebakken vis met saus</t>
-  </si>
-  <si>
-    <t>loempia speciaal</t>
-  </si>
-  <si>
-    <t>kerriesoep</t>
-  </si>
-  <si>
-    <t>bospaddestoelensoep</t>
-  </si>
-  <si>
-    <t>vermicellisoep</t>
-  </si>
-  <si>
-    <t>chinese bamisoep</t>
-  </si>
-  <si>
-    <t>indiase tandoorisoep</t>
-  </si>
-  <si>
-    <t>tomatensoep met runder gehakt balletjes</t>
-  </si>
-  <si>
-    <t>kippensoep met pistolet kruiden boter</t>
-  </si>
-  <si>
-    <t>erwtensoep met roggebrood/katenspek</t>
+    <t>Pasen, gesloten </t>
+  </si>
+  <si>
+    <t> Wrap roomkaas, runderrookvlees en ei</t>
+  </si>
+  <si>
+    <t>Ambachtelijk gebakken broodje huisgebraden gehakt </t>
+  </si>
+  <si>
+    <t>Ambachtelijk gebakken broodje ossenworst met mosterd en augurk </t>
+  </si>
+  <si>
+    <t> Ambachtelijk gebakken broodje Brugse beenham</t>
+  </si>
+  <si>
+    <t>Pasen, gesloten  </t>
+  </si>
+  <si>
+    <t>Ambachtelijk gebakken broodje Old Amsterdam</t>
+  </si>
+  <si>
+    <t>Ambachtelijk gebakken broodje zwarte peper kaas </t>
+  </si>
+  <si>
+    <t> Ambachtelijk gebakken broodje walnotenkaas</t>
+  </si>
+  <si>
+    <t>Ambachtelijk gebakken broodje Tomaten-Olijvenkaas </t>
+  </si>
+  <si>
+    <t> Tre formaggi</t>
+  </si>
+  <si>
+    <t>Spinata Romana, kaas en tomaat </t>
+  </si>
+  <si>
+    <t>Ham en kaas </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> € 1.49 </t>
+  </si>
+  <si>
+    <t>Omelet van de plaat </t>
+  </si>
+  <si>
+    <t>Kipsate met passend garnituur </t>
+  </si>
+  <si>
+    <t>Loempia speciaal </t>
+  </si>
+  <si>
+    <t> Gebakken kibbeling met saus</t>
+  </si>
+  <si>
+    <t>Groentebouillon </t>
+  </si>
+  <si>
+    <t> Rundvleesbouillon</t>
+  </si>
+  <si>
+    <t>Bospaddestoelen </t>
+  </si>
+  <si>
+    <t>Kruidenbouillon </t>
+  </si>
+  <si>
+    <t> Special</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Vismarkt</t>
+  </si>
+  <si>
+    <t>Heldere kippensoep </t>
+  </si>
+  <si>
+    <t>Champignonsoep </t>
+  </si>
+  <si>
+    <t>Tomaten-Crèmesoep </t>
+  </si>
+  <si>
+    <t>Kerriesoep</t>
+  </si>
+  <si>
+    <t>week 15 van 6 april t/m 10 april 2015.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;€&quot;\ #,##0.00_-;[Red]&quot;€&quot;\ #,##0.00\-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * #,##0.00\-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <name val="Arial"/>
@@ -408,8 +383,21 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF17375D"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF17375D"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
-      <color theme="3" tint="-0.249977111117893"/>
+      <color rgb="FF17375D"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -422,7 +410,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -460,6 +448,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FF376091"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF376091"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF376091"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FF376091"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color rgb="FF376091"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF376091"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FF376091"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FF376091"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF376091"/>
+      </right>
+      <top/>
+      <bottom style="mediumDashed">
+        <color rgb="FF376091"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color rgb="FF376091"/>
+      </right>
+      <top/>
+      <bottom style="mediumDashed">
+        <color rgb="FF376091"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color rgb="FF376091"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FF376091"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF376091"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF376091"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -477,7 +539,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -502,25 +564,49 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -837,361 +923,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.77734375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.77734375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.77734375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="15.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.77734375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.21875" style="12" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A1" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
+      <c r="A1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="12" customHeight="1" thickBot="1"/>
     <row r="3" spans="1:11" s="5" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="14"/>
-    </row>
-    <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A4" s="6" t="s">
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" ht="43.5" customHeight="1" thickBot="1">
+      <c r="A4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="19">
+        <v>3.49</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="19">
+        <v>3.49</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="19">
+        <v>3.49</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="19">
+        <v>3.49</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="19">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="26">
+        <v>3.49</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="26">
+        <v>3.49</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="26">
+        <v>3.49</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="20">
+        <v>3.49</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="20">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="29.25" customHeight="1" thickBot="1">
+      <c r="A6" s="23"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="19">
+        <v>1.79</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="19">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="20">
+        <v>3.25</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="20">
+        <v>3.25</v>
+      </c>
+      <c r="F7" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="G7" s="20">
+        <v>3.25</v>
+      </c>
+      <c r="H7" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="I7" s="20">
+        <v>3.25</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="20">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="27" customHeight="1" thickBot="1">
+      <c r="A8" s="23"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="19">
+        <v>1.65</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="19">
+        <v>1.65</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="19">
+        <v>1.65</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="19">
+        <v>1.65</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="19">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="39" customHeight="1" thickBot="1">
+      <c r="A9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="19">
+        <v>2.99</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="19">
+        <v>2.99</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="19">
+        <v>2.99</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="19">
+        <v>2.99</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="7" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="44.25" customHeight="1" thickBot="1">
+      <c r="A10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="19">
+        <v>3.75</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="7" t="s">
+      <c r="E10" s="19">
+        <v>3.75</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="G10" s="19">
+        <v>3.75</v>
+      </c>
+      <c r="H10" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="I10" s="19">
+        <v>2.75</v>
+      </c>
+      <c r="J10" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="K10" s="19">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="48.75" customHeight="1" thickBot="1">
+      <c r="A11" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="18" t="s">
+      <c r="E11" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="G11" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="45.75" customHeight="1" thickBot="1">
+      <c r="A12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="C12" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="13.5" thickBot="1">
+      <c r="A13" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="7" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="15">
-        <v>2.99</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="15">
-        <v>2.99</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="15">
-        <v>2.99</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="15">
-        <v>2.99</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K9" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="16">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="16">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" s="16">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="I10" s="16">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="K10" s="16">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="59.25" customHeight="1" thickBot="1">
-      <c r="A11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="15">
-        <v>3.75</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="K11" s="16"/>
-    </row>
-    <row r="12" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="17"/>
+      <c r="K13" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="16">
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -1252,34 +1366,34 @@
         <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="K2" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
@@ -1287,34 +1401,34 @@
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
@@ -1322,65 +1436,65 @@
         <v>6</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
@@ -1388,34 +1502,34 @@
         <v>9</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="K6" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="45" customHeight="1" thickBot="1">
@@ -1423,58 +1537,58 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K8" s="9"/>
     </row>
@@ -1493,26 +1607,26 @@
     </row>
     <row r="10" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K10" s="7"/>
     </row>
@@ -1533,7 +1647,7 @@
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1543,6 +1657,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DDD0688C7F746241976DCC457AF9E441" ma:contentTypeVersion="1" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="4d7eea835347aa2e17a0375ea5e88588">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c231a323-207f-4e01-8e69-d5b78e73a55e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b47ee0df75d323c3aba661ef03bb5845" ns2:_="">
     <xsd:import namespace="c231a323-207f-4e01-8e69-d5b78e73a55e"/>
@@ -1682,22 +1811,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D614DA5-AECB-4D81-8F79-8BA71C923CBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9423B2A-D916-4158-A022-332E8F117717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4505940B-A38A-4016-B4F0-7361F40E32B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1713,21 +1844,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9423B2A-D916-4158-A022-332E8F117717}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D614DA5-AECB-4D81-8F79-8BA71C923CBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>